<commit_message>
added eslint, removed unused json, changed json to js array
</commit_message>
<xml_diff>
--- a/media/invoice-template.xlsx
+++ b/media/invoice-template.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="109">
   <si>
     <t>Your Payout</t>
   </si>
@@ -339,46 +339,16 @@
     <t>2022-03-06 10:12:12</t>
   </si>
   <si>
-    <t>384452632154</t>
-  </si>
-  <si>
     <t>delivered</t>
   </si>
   <si>
     <t>regular</t>
   </si>
   <si>
-    <t>0</t>
-  </si>
-  <si>
-    <t>45</t>
-  </si>
-  <si>
-    <t>47</t>
-  </si>
-  <si>
-    <t>345</t>
-  </si>
-  <si>
-    <t>69</t>
-  </si>
-  <si>
-    <t>6</t>
-  </si>
-  <si>
-    <t>4</t>
-  </si>
-  <si>
-    <t>24.0%</t>
-  </si>
-  <si>
-    <t>36</t>
-  </si>
-  <si>
-    <t>40</t>
-  </si>
-  <si>
-    <t>12</t>
+    <t>customer payable</t>
+  </si>
+  <si>
+    <t/>
   </si>
 </sst>
 </file>
@@ -396,7 +366,7 @@
       <b/>
       <sz val="30"/>
       <color rgb="FF000000"/>
-      <name val="Arial"/>
+      <name val="Roboto"/>
       <family val="1"/>
     </font>
     <font>
@@ -408,59 +378,59 @@
     <font>
       <sz val="15"/>
       <color rgb="FF000000"/>
-      <name val="Arial"/>
+      <name val="Roboto"/>
       <family val="1"/>
     </font>
     <font>
       <b/>
       <sz val="12"/>
       <color rgb="FF000000"/>
-      <name val="Arial"/>
+      <name val="Roboto"/>
       <family val="1"/>
     </font>
     <font>
       <b/>
       <sz val="15"/>
       <color rgb="FF086AD8"/>
-      <name val="Arial"/>
+      <name val="Roboto"/>
       <family val="1"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF1D1D1D"/>
-      <name val="Arial"/>
+      <name val="Roboto"/>
       <family val="1"/>
     </font>
     <font>
       <b/>
       <sz val="18"/>
       <color rgb="FF000000"/>
-      <name val="Arial"/>
+      <name val="Roboto"/>
       <family val="1"/>
     </font>
     <font>
       <b/>
       <sz val="15"/>
       <color rgb="FF000000"/>
-      <name val="Arial"/>
+      <name val="Roboto"/>
       <family val="1"/>
     </font>
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
-      <name val="Arial"/>
+      <name val="Roboto"/>
       <family val="1"/>
     </font>
     <font>
       <sz val="12"/>
       <color rgb="FF6A6A6A"/>
-      <name val="Arial"/>
+      <name val="Roboto"/>
       <family val="1"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
-      <name val="Arial"/>
+      <name val="Roboto"/>
       <family val="1"/>
     </font>
   </fonts>
@@ -532,7 +502,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="20">
     <xf applyFont="1" fontId="0"/>
     <xf applyFont="1" fontId="0" applyFill="1" fillId="2" applyBorder="1" borderId="1"/>
     <xf applyFont="1" fontId="1" applyBorder="1" borderId="1"/>
@@ -547,9 +517,6 @@
     </xf>
     <xf applyFont="1" fontId="5" applyBorder="1" borderId="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf applyFont="1" fontId="0" applyBorder="1" borderId="2" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf applyFont="1" fontId="6" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -648,33 +615,33 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="15" customHeight="1">
-      <c r="A1" s="16"/>
-      <c r="B1" s="16"/>
-      <c r="C1" s="16"/>
-      <c r="D1" s="16"/>
-      <c r="E1" s="16"/>
-      <c r="F1" s="16"/>
-      <c r="G1" s="16"/>
-      <c r="H1" s="16"/>
-      <c r="I1" s="16"/>
-      <c r="J1" s="16"/>
-      <c r="K1" s="16"/>
-      <c r="L1" s="16"/>
-      <c r="M1" s="16"/>
-      <c r="N1" s="16"/>
-      <c r="O1" s="16"/>
+      <c r="A1" s="15"/>
+      <c r="B1" s="15"/>
+      <c r="C1" s="15"/>
+      <c r="D1" s="15"/>
+      <c r="E1" s="15"/>
+      <c r="F1" s="15"/>
+      <c r="G1" s="15"/>
+      <c r="H1" s="15"/>
+      <c r="I1" s="15"/>
+      <c r="J1" s="15"/>
+      <c r="K1" s="15"/>
+      <c r="L1" s="15"/>
+      <c r="M1" s="15"/>
+      <c r="N1" s="15"/>
+      <c r="O1" s="15"/>
     </row>
     <row r="2" spans="1:15">
       <c r="A2" s="3"/>
-      <c r="B2" s="17"/>
-      <c r="C2" s="17"/>
-      <c r="D2" s="17"/>
-      <c r="E2" s="17"/>
-      <c r="F2" s="17"/>
-      <c r="G2" s="17"/>
-      <c r="H2" s="17"/>
-      <c r="I2" s="17"/>
-      <c r="J2" s="17"/>
+      <c r="B2" s="16"/>
+      <c r="C2" s="16"/>
+      <c r="D2" s="16"/>
+      <c r="E2" s="16"/>
+      <c r="F2" s="16"/>
+      <c r="G2" s="16"/>
+      <c r="H2" s="16"/>
+      <c r="I2" s="16"/>
+      <c r="J2" s="16"/>
       <c r="K2" s="3"/>
       <c r="L2" s="3"/>
       <c r="M2" s="3"/>
@@ -683,15 +650,15 @@
     </row>
     <row r="3" spans="1:15">
       <c r="A3" s="3"/>
-      <c r="B3" s="17"/>
-      <c r="C3" s="17"/>
-      <c r="D3" s="17"/>
-      <c r="E3" s="17"/>
-      <c r="F3" s="17"/>
-      <c r="G3" s="17"/>
-      <c r="H3" s="17"/>
-      <c r="I3" s="17"/>
-      <c r="J3" s="17"/>
+      <c r="B3" s="16"/>
+      <c r="C3" s="16"/>
+      <c r="D3" s="16"/>
+      <c r="E3" s="16"/>
+      <c r="F3" s="16"/>
+      <c r="G3" s="16"/>
+      <c r="H3" s="16"/>
+      <c r="I3" s="16"/>
+      <c r="J3" s="16"/>
       <c r="K3" s="3"/>
       <c r="L3" s="3"/>
       <c r="M3" s="3"/>
@@ -700,15 +667,15 @@
     </row>
     <row r="4" spans="1:15">
       <c r="A4" s="3"/>
-      <c r="B4" s="17"/>
-      <c r="C4" s="17"/>
-      <c r="D4" s="17"/>
-      <c r="E4" s="17"/>
-      <c r="F4" s="17"/>
-      <c r="G4" s="17"/>
-      <c r="H4" s="17"/>
-      <c r="I4" s="17"/>
-      <c r="J4" s="17"/>
+      <c r="B4" s="16"/>
+      <c r="C4" s="16"/>
+      <c r="D4" s="16"/>
+      <c r="E4" s="16"/>
+      <c r="F4" s="16"/>
+      <c r="G4" s="16"/>
+      <c r="H4" s="16"/>
+      <c r="I4" s="16"/>
+      <c r="J4" s="16"/>
       <c r="K4" s="3"/>
       <c r="L4" s="3"/>
       <c r="M4" s="3"/>
@@ -768,7 +735,7 @@
     </row>
     <row r="8" spans="1:15">
       <c r="A8" s="3"/>
-      <c r="B8" s="17" t="s">
+      <c r="B8" s="16" t="s">
         <v>0</v>
       </c>
       <c r="C8" s="3"/>
@@ -804,7 +771,7 @@
     </row>
     <row r="10" spans="1:15">
       <c r="A10" s="3"/>
-      <c r="B10" s="18" t="s">
+      <c r="B10" s="17" t="s">
         <v>1</v>
       </c>
       <c r="C10" s="3"/>
@@ -914,10 +881,10 @@
     </row>
     <row r="16" spans="1:15">
       <c r="A16" s="3"/>
-      <c r="B16" s="12" t="s">
+      <c r="B16" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="C16" s="12" t="s">
+      <c r="C16" s="11" t="s">
         <v>6</v>
       </c>
       <c r="D16" s="3"/>
@@ -935,10 +902,10 @@
     </row>
     <row r="17" spans="1:15" ht="20" customHeight="1">
       <c r="A17" s="3"/>
-      <c r="B17" s="19" t="s">
+      <c r="B17" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="C17" s="19" t="s">
+      <c r="C17" s="18" t="s">
         <v>8</v>
       </c>
       <c r="D17" s="3"/>
@@ -1007,10 +974,10 @@
     </row>
     <row r="21" spans="1:15">
       <c r="A21" s="3"/>
-      <c r="B21" s="12" t="s">
+      <c r="B21" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="C21" s="12" t="s">
+      <c r="C21" s="11" t="s">
         <v>10</v>
       </c>
       <c r="D21" s="3"/>
@@ -1028,10 +995,10 @@
     </row>
     <row r="22" spans="1:15">
       <c r="A22" s="3"/>
-      <c r="B22" s="19" t="s">
+      <c r="B22" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="C22" s="19" t="s">
+      <c r="C22" s="18" t="s">
         <v>12</v>
       </c>
       <c r="D22" s="3"/>
@@ -1117,10 +1084,10 @@
     </row>
     <row r="27" spans="1:15">
       <c r="A27" s="3"/>
-      <c r="B27" s="19" t="s">
+      <c r="B27" s="18" t="s">
         <v>13</v>
       </c>
-      <c r="C27" s="19"/>
+      <c r="C27" s="18"/>
       <c r="D27" s="3"/>
       <c r="E27" s="3"/>
       <c r="F27" s="3"/>
@@ -1136,10 +1103,10 @@
     </row>
     <row r="28" spans="1:15">
       <c r="A28" s="3"/>
-      <c r="B28" s="12" t="s">
+      <c r="B28" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="C28" s="12"/>
+      <c r="C28" s="11"/>
       <c r="D28" s="3"/>
       <c r="E28" s="3"/>
       <c r="F28" s="3"/>
@@ -1189,10 +1156,10 @@
     </row>
     <row r="31" spans="1:15">
       <c r="A31" s="3"/>
-      <c r="B31" s="20" t="s">
+      <c r="B31" s="19" t="s">
         <v>15</v>
       </c>
-      <c r="C31" s="20"/>
+      <c r="C31" s="19"/>
       <c r="D31" s="3"/>
       <c r="E31" s="3"/>
       <c r="F31" s="3"/>
@@ -1208,10 +1175,10 @@
     </row>
     <row r="32" spans="1:15" ht="30" customHeight="1">
       <c r="A32" s="3"/>
-      <c r="B32" s="12" t="s">
+      <c r="B32" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="C32" s="12"/>
+      <c r="C32" s="11"/>
       <c r="D32" s="3"/>
       <c r="E32" s="3"/>
       <c r="F32" s="3"/>
@@ -1244,10 +1211,10 @@
     </row>
     <row r="34" spans="1:15">
       <c r="A34" s="3"/>
-      <c r="B34" s="20" t="s">
+      <c r="B34" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="C34" s="20"/>
+      <c r="C34" s="19"/>
       <c r="D34" s="3"/>
       <c r="E34" s="3"/>
       <c r="F34" s="3"/>
@@ -1299,10 +1266,10 @@
     </row>
     <row r="37" spans="1:15">
       <c r="A37" s="3"/>
-      <c r="B37" s="20" t="s">
+      <c r="B37" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="C37" s="20"/>
+      <c r="C37" s="19"/>
       <c r="D37" s="3"/>
       <c r="E37" s="3"/>
       <c r="F37" s="3"/>
@@ -1318,10 +1285,10 @@
     </row>
     <row r="38" spans="1:15" ht="30" customHeight="1">
       <c r="A38" s="3"/>
-      <c r="B38" s="12" t="s">
+      <c r="B38" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="C38" s="12"/>
+      <c r="C38" s="11"/>
       <c r="D38" s="3"/>
       <c r="E38" s="3"/>
       <c r="F38" s="3"/>
@@ -1354,10 +1321,10 @@
     </row>
     <row r="40" spans="1:15">
       <c r="A40" s="3"/>
-      <c r="B40" s="20" t="s">
+      <c r="B40" s="19" t="s">
         <v>21</v>
       </c>
-      <c r="C40" s="20"/>
+      <c r="C40" s="19"/>
       <c r="D40" s="3"/>
       <c r="E40" s="3"/>
       <c r="F40" s="3"/>
@@ -1373,10 +1340,10 @@
     </row>
     <row r="41" spans="1:15" ht="30" customHeight="1">
       <c r="A41" s="3"/>
-      <c r="B41" s="12" t="s">
+      <c r="B41" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="C41" s="12"/>
+      <c r="C41" s="11"/>
       <c r="D41" s="3"/>
       <c r="E41" s="3"/>
       <c r="F41" s="3"/>
@@ -1409,10 +1376,10 @@
     </row>
     <row r="43" spans="1:15">
       <c r="A43" s="3"/>
-      <c r="B43" s="20" t="s">
+      <c r="B43" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="C43" s="20"/>
+      <c r="C43" s="19"/>
       <c r="D43" s="3"/>
       <c r="E43" s="3"/>
       <c r="F43" s="3"/>
@@ -1428,10 +1395,10 @@
     </row>
     <row r="44" spans="1:15" ht="30" customHeight="1">
       <c r="A44" s="3"/>
-      <c r="B44" s="12" t="s">
+      <c r="B44" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="C44" s="12"/>
+      <c r="C44" s="11"/>
       <c r="D44" s="3"/>
       <c r="E44" s="3"/>
       <c r="F44" s="3"/>
@@ -2440,7 +2407,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
-      <c r="A1" s="16"/>
+      <c r="A1" s="15"/>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
@@ -2469,7 +2436,7 @@
     </row>
     <row r="4" spans="1:6" ht="50" customHeight="1">
       <c r="A4" s="3"/>
-      <c r="B4" s="17" t="s">
+      <c r="B4" s="16" t="s">
         <v>15</v>
       </c>
       <c r="C4" s="3"/>
@@ -2509,114 +2476,114 @@
     </row>
     <row r="8" spans="1:6" ht="20" customHeight="1">
       <c r="A8" s="3"/>
-      <c r="B8" s="11" t="s">
+      <c r="B8" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="C8" s="14" t="s">
+      <c r="C8" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="D8" s="14" t="s">
+      <c r="D8" s="13" t="s">
         <v>40</v>
       </c>
-      <c r="E8" s="14" t="s">
+      <c r="E8" s="13" t="s">
         <v>12</v>
       </c>
       <c r="F8" s="0"/>
     </row>
     <row r="9" spans="1:6" ht="20" customHeight="1">
       <c r="A9" s="3"/>
-      <c r="B9" s="11" t="s">
+      <c r="B9" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="C9" s="14" t="s">
+      <c r="C9" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="D9" s="14" t="s">
+      <c r="D9" s="13" t="s">
         <v>41</v>
       </c>
-      <c r="E9" s="14" t="s">
+      <c r="E9" s="13" t="s">
         <v>44</v>
       </c>
       <c r="F9" s="0"/>
     </row>
     <row r="10" spans="1:6" ht="30" customHeight="1">
       <c r="A10" s="3"/>
-      <c r="B10" s="11" t="s">
+      <c r="B10" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="C10" s="14" t="s">
+      <c r="C10" s="13" t="s">
         <v>36</v>
       </c>
-      <c r="D10" s="14" t="s">
+      <c r="D10" s="13" t="s">
         <v>36</v>
       </c>
-      <c r="E10" s="14" t="s">
+      <c r="E10" s="13" t="s">
         <v>36</v>
       </c>
       <c r="F10" s="0"/>
     </row>
     <row r="11" spans="1:6" ht="20" customHeight="1">
       <c r="A11" s="3"/>
-      <c r="B11" s="11" t="s">
+      <c r="B11" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="C11" s="14" t="s">
+      <c r="C11" s="13" t="s">
         <v>37</v>
       </c>
-      <c r="D11" s="14" t="s">
+      <c r="D11" s="13" t="s">
         <v>42</v>
       </c>
-      <c r="E11" s="14" t="s">
+      <c r="E11" s="13" t="s">
         <v>45</v>
       </c>
       <c r="F11" s="0"/>
     </row>
     <row r="12" spans="1:6" ht="20" customHeight="1">
       <c r="A12" s="3"/>
-      <c r="B12" s="11" t="s">
+      <c r="B12" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="C12" s="14" t="s">
+      <c r="C12" s="13" t="s">
         <v>38</v>
       </c>
-      <c r="D12" s="14" t="s">
+      <c r="D12" s="13" t="s">
         <v>43</v>
       </c>
-      <c r="E12" s="14" t="s">
+      <c r="E12" s="13" t="s">
         <v>46</v>
       </c>
       <c r="F12" s="0"/>
     </row>
     <row r="13" spans="1:6" ht="20" customHeight="1">
       <c r="A13" s="3"/>
-      <c r="B13" s="11" t="s">
+      <c r="B13" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="C13" s="14" t="s">
+      <c r="C13" s="13" t="s">
         <v>39</v>
       </c>
-      <c r="D13" s="14" t="s">
+      <c r="D13" s="13" t="s">
         <v>36</v>
       </c>
-      <c r="E13" s="14" t="s">
+      <c r="E13" s="13" t="s">
         <v>47</v>
       </c>
       <c r="F13" s="0"/>
     </row>
     <row r="14" spans="1:6" ht="30" customHeight="1">
-      <c r="A14" s="18" t="s">
+      <c r="A14" s="17" t="s">
         <v>48</v>
       </c>
       <c r="B14" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="C14" s="14" t="s">
+      <c r="C14" s="13" t="s">
         <v>50</v>
       </c>
-      <c r="D14" s="14" t="s">
+      <c r="D14" s="13" t="s">
         <v>43</v>
       </c>
-      <c r="E14" s="14" t="s">
+      <c r="E14" s="13" t="s">
         <v>51</v>
       </c>
       <c r="F14" s="0"/>
@@ -2639,129 +2606,129 @@
     </row>
     <row r="17" spans="1:6" ht="20" customHeight="1">
       <c r="A17" s="3"/>
-      <c r="B17" s="11" t="s">
+      <c r="B17" s="10" t="s">
         <v>52</v>
       </c>
-      <c r="C17" s="14" t="s">
+      <c r="C17" s="13" t="s">
         <v>60</v>
       </c>
-      <c r="D17" s="14" t="s">
+      <c r="D17" s="13" t="s">
         <v>36</v>
       </c>
-      <c r="E17" s="14" t="s">
+      <c r="E17" s="13" t="s">
         <v>63</v>
       </c>
       <c r="F17" s="0"/>
     </row>
     <row r="18" spans="1:6" ht="20" customHeight="1">
       <c r="A18" s="3"/>
-      <c r="B18" s="11" t="s">
+      <c r="B18" s="10" t="s">
         <v>53</v>
       </c>
-      <c r="C18" s="14" t="s">
+      <c r="C18" s="13" t="s">
         <v>36</v>
       </c>
-      <c r="D18" s="14" t="s">
+      <c r="D18" s="13" t="s">
         <v>36</v>
       </c>
-      <c r="E18" s="14" t="s">
+      <c r="E18" s="13" t="s">
         <v>36</v>
       </c>
       <c r="F18" s="0"/>
     </row>
     <row r="19" spans="1:6" ht="20" customHeight="1">
       <c r="A19" s="3"/>
-      <c r="B19" s="11" t="s">
+      <c r="B19" s="10" t="s">
         <v>54</v>
       </c>
-      <c r="C19" s="14" t="s">
+      <c r="C19" s="13" t="s">
         <v>36</v>
       </c>
-      <c r="D19" s="14" t="s">
+      <c r="D19" s="13" t="s">
         <v>36</v>
       </c>
-      <c r="E19" s="14" t="s">
+      <c r="E19" s="13" t="s">
         <v>36</v>
       </c>
       <c r="F19" s="0"/>
     </row>
     <row r="20" spans="1:6" ht="20" customHeight="1">
       <c r="A20" s="3"/>
-      <c r="B20" s="11" t="s">
+      <c r="B20" s="10" t="s">
         <v>55</v>
       </c>
-      <c r="C20" s="14" t="s">
+      <c r="C20" s="13" t="s">
         <v>36</v>
       </c>
-      <c r="D20" s="14" t="s">
+      <c r="D20" s="13" t="s">
         <v>36</v>
       </c>
-      <c r="E20" s="14" t="s">
+      <c r="E20" s="13" t="s">
         <v>36</v>
       </c>
       <c r="F20" s="0"/>
     </row>
     <row r="21" spans="2:6" ht="20" customHeight="1">
-      <c r="B21" s="11" t="s">
+      <c r="B21" s="10" t="s">
         <v>56</v>
       </c>
-      <c r="C21" s="14" t="s">
+      <c r="C21" s="13" t="s">
         <v>36</v>
       </c>
-      <c r="D21" s="14" t="s">
+      <c r="D21" s="13" t="s">
         <v>36</v>
       </c>
-      <c r="E21" s="14" t="s">
+      <c r="E21" s="13" t="s">
         <v>36</v>
       </c>
-      <c r="F21" s="15"/>
+      <c r="F21" s="14"/>
     </row>
     <row r="22" spans="1:6" ht="20" customHeight="1">
-      <c r="A22" s="15"/>
-      <c r="B22" s="11" t="s">
+      <c r="A22" s="14"/>
+      <c r="B22" s="10" t="s">
         <v>57</v>
       </c>
-      <c r="C22" s="14" t="s">
+      <c r="C22" s="13" t="s">
         <v>36</v>
       </c>
-      <c r="D22" s="14" t="s">
+      <c r="D22" s="13" t="s">
         <v>36</v>
       </c>
-      <c r="E22" s="14" t="s">
+      <c r="E22" s="13" t="s">
         <v>36</v>
       </c>
-      <c r="F22" s="15"/>
+      <c r="F22" s="14"/>
     </row>
     <row r="23" spans="2:6" ht="30" customHeight="1">
-      <c r="B23" s="11" t="s">
+      <c r="B23" s="10" t="s">
         <v>58</v>
       </c>
-      <c r="C23" s="14" t="s">
+      <c r="C23" s="13" t="s">
         <v>61</v>
       </c>
-      <c r="D23" s="14" t="s">
+      <c r="D23" s="13" t="s">
         <v>36</v>
       </c>
-      <c r="E23" s="14" t="s">
+      <c r="E23" s="13" t="s">
         <v>64</v>
       </c>
-      <c r="F23" s="15"/>
+      <c r="F23" s="14"/>
     </row>
     <row r="24" spans="1:6" ht="30" customHeight="1">
-      <c r="A24" s="15"/>
-      <c r="B24" s="11" t="s">
+      <c r="A24" s="14"/>
+      <c r="B24" s="10" t="s">
         <v>59</v>
       </c>
-      <c r="C24" s="14" t="s">
+      <c r="C24" s="13" t="s">
         <v>62</v>
       </c>
-      <c r="D24" s="14" t="s">
+      <c r="D24" s="13" t="s">
         <v>36</v>
       </c>
-      <c r="E24" s="14" t="s">
+      <c r="E24" s="13" t="s">
         <v>65</v>
       </c>
-      <c r="F24" s="15"/>
+      <c r="F24" s="14"/>
     </row>
     <row r="25" spans="1:6" ht="30" customHeight="1">
       <c r="A25" s="4" t="s">
@@ -2770,24 +2737,24 @@
       <c r="B25" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="C25" s="14" t="s">
+      <c r="C25" s="13" t="s">
         <v>67</v>
       </c>
-      <c r="D25" s="14" t="s">
+      <c r="D25" s="13" t="s">
         <v>36</v>
       </c>
-      <c r="E25" s="14" t="s">
+      <c r="E25" s="13" t="s">
         <v>68</v>
       </c>
-      <c r="F25" s="15"/>
+      <c r="F25" s="14"/>
     </row>
     <row r="26" spans="1:6" ht="800" customHeight="1">
-      <c r="A26" s="15"/>
-      <c r="B26" s="15"/>
-      <c r="C26" s="15"/>
-      <c r="D26" s="15"/>
-      <c r="E26" s="15"/>
-      <c r="F26" s="15"/>
+      <c r="A26" s="14"/>
+      <c r="B26" s="14"/>
+      <c r="C26" s="14"/>
+      <c r="D26" s="14"/>
+      <c r="E26" s="14"/>
+      <c r="F26" s="14"/>
     </row>
     <row r="27" ht="20" customHeight="1"/>
     <row r="28" ht="20" customHeight="1"/>
@@ -2921,7 +2888,7 @@
       <c r="AT1" s="1"/>
       <c r="AU1" s="1"/>
     </row>
-    <row r="2" spans="1:28">
+    <row r="2" spans="1:28" ht="30" customHeight="1">
       <c r="A2" s="5" t="s">
         <v>70</v>
       </c>
@@ -2958,359 +2925,350 @@
       <c r="AB2" s="5"/>
     </row>
     <row r="3" spans="1:32" ht="60" customHeight="1">
-      <c r="A3" s="8" t="s">
+      <c r="A3" s="7" t="s">
         <v>73</v>
       </c>
-      <c r="B3" s="8" t="s">
+      <c r="B3" s="7" t="s">
         <v>74</v>
       </c>
-      <c r="C3" s="8" t="s">
+      <c r="C3" s="7" t="s">
         <v>75</v>
       </c>
-      <c r="D3" s="8" t="s">
+      <c r="D3" s="7" t="s">
         <v>76</v>
       </c>
-      <c r="E3" s="8" t="s">
+      <c r="E3" s="7" t="s">
         <v>78</v>
       </c>
-      <c r="F3" s="8" t="s">
+      <c r="F3" s="7" t="s">
         <v>77</v>
       </c>
-      <c r="G3" s="8" t="s">
+      <c r="G3" s="7" t="s">
         <v>79</v>
       </c>
-      <c r="H3" s="8" t="s">
+      <c r="H3" s="7" t="s">
         <v>80</v>
       </c>
-      <c r="I3" s="8" t="s">
+      <c r="I3" s="7" t="s">
         <v>81</v>
       </c>
-      <c r="J3" s="8" t="s">
+      <c r="J3" s="7" t="s">
         <v>82</v>
       </c>
-      <c r="K3" s="8" t="s">
+      <c r="K3" s="7" t="s">
         <v>83</v>
       </c>
-      <c r="L3" s="8" t="s">
+      <c r="L3" s="7" t="s">
         <v>84</v>
       </c>
-      <c r="M3" s="13" t="s">
+      <c r="M3" s="12" t="s">
         <v>85</v>
       </c>
-      <c r="N3" s="8" t="s">
+      <c r="N3" s="7" t="s">
         <v>73</v>
       </c>
-      <c r="O3" s="8" t="s">
+      <c r="O3" s="7" t="s">
         <v>86</v>
       </c>
-      <c r="P3" s="8" t="s">
+      <c r="P3" s="7" t="s">
         <v>87</v>
       </c>
-      <c r="Q3" s="8" t="s">
+      <c r="Q3" s="7" t="s">
         <v>88</v>
       </c>
-      <c r="R3" s="8" t="s">
+      <c r="R3" s="7" t="s">
         <v>89</v>
       </c>
-      <c r="S3" s="8" t="s">
+      <c r="S3" s="7" t="s">
         <v>90</v>
       </c>
-      <c r="T3" s="8" t="s">
+      <c r="T3" s="7" t="s">
         <v>91</v>
       </c>
-      <c r="U3" s="8" t="s">
+      <c r="U3" s="7" t="s">
         <v>92</v>
       </c>
-      <c r="V3" s="8" t="s">
+      <c r="V3" s="7" t="s">
         <v>93</v>
       </c>
-      <c r="W3" s="8" t="s">
+      <c r="W3" s="7" t="s">
         <v>94</v>
       </c>
-      <c r="X3" s="8" t="s">
+      <c r="X3" s="7" t="s">
         <v>95</v>
       </c>
-      <c r="Y3" s="13" t="s">
+      <c r="Y3" s="12" t="s">
         <v>96</v>
       </c>
-      <c r="Z3" s="8" t="s">
+      <c r="Z3" s="7" t="s">
         <v>97</v>
       </c>
-      <c r="AA3" s="8" t="s">
+      <c r="AA3" s="7" t="s">
         <v>98</v>
       </c>
-      <c r="AB3" s="8" t="s">
+      <c r="AB3" s="7" t="s">
         <v>99</v>
       </c>
-      <c r="AC3" s="8" t="s">
+      <c r="AC3" s="7" t="s">
         <v>100</v>
       </c>
-      <c r="AD3" s="8" t="s">
+      <c r="AD3" s="7" t="s">
         <v>101</v>
       </c>
-      <c r="AE3" s="13" t="s">
+      <c r="AE3" s="12" t="s">
         <v>102</v>
       </c>
-      <c r="AF3" s="8" t="s">
+      <c r="AF3" s="7" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="4" spans="1:29">
+    <row r="4" spans="1:27">
       <c r="A4" s="7" t="s">
         <v>104</v>
       </c>
-      <c r="B4" s="7" t="s">
+      <c r="B4" s="7" t="n">
+        <v>384410695125</v>
+      </c>
+      <c r="C4" s="7" t="s">
         <v>105</v>
       </c>
-      <c r="C4" s="7" t="s">
+      <c r="D4" s="7" t="s">
         <v>106</v>
       </c>
-      <c r="D4" s="7" t="s">
+      <c r="E4" s="7" t="n">
+        <v>150</v>
+      </c>
+      <c r="F4" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="G4" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="H4" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="I4" s="7" t="n">
+        <v>24</v>
+      </c>
+      <c r="J4" s="7" t="n">
+        <v>174</v>
+      </c>
+      <c r="K4" s="7" t="s">
         <v>107</v>
       </c>
-      <c r="F4" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="G4" s="7" t="s">
-        <v>108</v>
-      </c>
-      <c r="H4" s="7" t="s">
-        <v>108</v>
-      </c>
-      <c r="I4" s="7" t="s">
-        <v>108</v>
-      </c>
-      <c r="J4" s="7" t="s">
-        <v>108</v>
-      </c>
-      <c r="K4" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="L4" s="7" t="s">
-        <v>108</v>
-      </c>
-      <c r="M4" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="N4" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="O4" s="7" t="s">
-        <v>115</v>
-      </c>
-      <c r="P4" s="7" t="s">
-        <v>116</v>
-      </c>
-      <c r="Q4" s="7" t="s">
-        <v>108</v>
-      </c>
-      <c r="R4" s="7" t="s">
-        <v>108</v>
-      </c>
-      <c r="S4" s="7" t="s">
-        <v>108</v>
-      </c>
-      <c r="T4" s="7" t="s">
-        <v>108</v>
-      </c>
-      <c r="U4" s="7" t="s">
-        <v>108</v>
-      </c>
-      <c r="V4" s="7" t="s">
-        <v>116</v>
-      </c>
-      <c r="W4" s="7" t="s">
-        <v>113</v>
-      </c>
-      <c r="X4" s="7" t="s">
-        <v>117</v>
+      <c r="L4" s="7" t="n">
+        <v>24</v>
+      </c>
+      <c r="M4" s="7" t="n">
+        <v>36</v>
+      </c>
+      <c r="N4" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="O4" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="P4" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q4" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="R4" s="7" t="n">
+        <v>6</v>
+      </c>
+      <c r="S4" s="7" t="n">
+        <v>42</v>
+      </c>
+      <c r="T4" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="U4" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="V4" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="W4" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="X4" s="7" t="n">
+        <v>0</v>
       </c>
       <c r="Y4" s="7" t="s">
         <v>108</v>
       </c>
-      <c r="Z4" s="7" t="s">
-        <v>108</v>
-      </c>
-      <c r="AA4" s="7" t="s">
-        <v>108</v>
-      </c>
-      <c r="AB4" s="7" t="s">
-        <v>113</v>
-      </c>
-      <c r="AC4" s="7" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="5" spans="1:29">
+      <c r="Z4" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA4" s="7" t="n">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="5" spans="1:27">
       <c r="A5" s="7" t="s">
         <v>104</v>
       </c>
-      <c r="B5" s="7" t="s">
+      <c r="B5" s="7" t="n">
+        <v>384410695125</v>
+      </c>
+      <c r="C5" s="7" t="s">
         <v>105</v>
       </c>
-      <c r="C5" s="7" t="s">
+      <c r="D5" s="7" t="s">
         <v>106</v>
       </c>
-      <c r="D5" s="7" t="s">
+      <c r="E5" s="7" t="n">
+        <v>150</v>
+      </c>
+      <c r="F5" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="G5" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="H5" s="7" t="n">
+        <v>45</v>
+      </c>
+      <c r="I5" s="7" t="n">
+        <v>24</v>
+      </c>
+      <c r="J5" s="7" t="n">
+        <v>399</v>
+      </c>
+      <c r="K5" s="7" t="s">
         <v>107</v>
       </c>
-      <c r="F5" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="G5" s="7" t="s">
-        <v>108</v>
-      </c>
-      <c r="H5" s="7" t="s">
-        <v>109</v>
-      </c>
-      <c r="I5" s="7" t="s">
-        <v>108</v>
-      </c>
-      <c r="J5" s="7" t="s">
-        <v>110</v>
-      </c>
-      <c r="K5" s="7" t="s">
-        <v>111</v>
-      </c>
-      <c r="L5" s="7" t="s">
-        <v>113</v>
-      </c>
-      <c r="M5" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="N5" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="O5" s="7" t="s">
-        <v>115</v>
-      </c>
-      <c r="P5" s="7" t="s">
-        <v>116</v>
-      </c>
-      <c r="Q5" s="7" t="s">
-        <v>108</v>
-      </c>
-      <c r="R5" s="7" t="s">
-        <v>108</v>
-      </c>
-      <c r="S5" s="7" t="s">
-        <v>108</v>
-      </c>
-      <c r="T5" s="7" t="s">
-        <v>108</v>
-      </c>
-      <c r="U5" s="7" t="s">
-        <v>108</v>
-      </c>
-      <c r="V5" s="7" t="s">
-        <v>116</v>
-      </c>
-      <c r="W5" s="7" t="s">
-        <v>113</v>
-      </c>
-      <c r="X5" s="7" t="s">
-        <v>117</v>
+      <c r="L5" s="7" t="n">
+        <v>24</v>
+      </c>
+      <c r="M5" s="7" t="n">
+        <v>36</v>
+      </c>
+      <c r="N5" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="O5" s="7" t="n">
+        <v>6</v>
+      </c>
+      <c r="P5" s="7" t="n">
+        <v>150</v>
+      </c>
+      <c r="Q5" s="7" t="n">
+        <v>150</v>
+      </c>
+      <c r="R5" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="S5" s="7" t="n">
+        <v>42</v>
+      </c>
+      <c r="T5" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="U5" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="V5" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="W5" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="X5" s="7" t="n">
+        <v>0</v>
       </c>
       <c r="Y5" s="7" t="s">
         <v>108</v>
       </c>
-      <c r="Z5" s="7" t="s">
-        <v>108</v>
-      </c>
-      <c r="AA5" s="7" t="s">
-        <v>108</v>
-      </c>
-      <c r="AB5" s="7" t="s">
-        <v>118</v>
-      </c>
-      <c r="AC5" s="7" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="6" spans="1:29">
+      <c r="Z5" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA5" s="7" t="n">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="6" spans="1:27">
       <c r="A6" s="7" t="s">
         <v>104</v>
       </c>
-      <c r="B6" s="7" t="s">
+      <c r="B6" s="7" t="n">
+        <v>384410695125</v>
+      </c>
+      <c r="C6" s="7" t="s">
         <v>105</v>
       </c>
-      <c r="C6" s="7" t="s">
+      <c r="D6" s="7" t="s">
         <v>106</v>
       </c>
-      <c r="D6" s="7" t="s">
+      <c r="E6" s="7" t="n">
+        <v>150</v>
+      </c>
+      <c r="F6" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="G6" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="H6" s="7" t="n">
+        <v>45</v>
+      </c>
+      <c r="I6" s="7" t="n">
+        <v>24</v>
+      </c>
+      <c r="J6" s="7" t="n">
+        <v>399</v>
+      </c>
+      <c r="K6" s="7" t="s">
         <v>107</v>
       </c>
-      <c r="F6" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="G6" s="7" t="s">
-        <v>108</v>
-      </c>
-      <c r="H6" s="7" t="s">
-        <v>108</v>
-      </c>
-      <c r="I6" s="7" t="s">
-        <v>108</v>
-      </c>
-      <c r="J6" s="7" t="s">
-        <v>108</v>
-      </c>
-      <c r="K6" s="7" t="s">
-        <v>112</v>
-      </c>
-      <c r="L6" s="7" t="s">
-        <v>114</v>
-      </c>
-      <c r="M6" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="N6" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="O6" s="7" t="s">
-        <v>115</v>
-      </c>
-      <c r="P6" s="7" t="s">
-        <v>116</v>
-      </c>
-      <c r="Q6" s="7" t="s">
-        <v>108</v>
-      </c>
-      <c r="R6" s="7" t="s">
-        <v>108</v>
-      </c>
-      <c r="S6" s="7" t="s">
-        <v>108</v>
-      </c>
-      <c r="T6" s="7" t="s">
-        <v>108</v>
-      </c>
-      <c r="U6" s="7" t="s">
-        <v>108</v>
-      </c>
-      <c r="V6" s="7" t="s">
-        <v>116</v>
-      </c>
-      <c r="W6" s="7" t="s">
-        <v>113</v>
-      </c>
-      <c r="X6" s="7" t="s">
-        <v>117</v>
+      <c r="L6" s="7" t="n">
+        <v>24</v>
+      </c>
+      <c r="M6" s="7" t="n">
+        <v>36</v>
+      </c>
+      <c r="N6" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="O6" s="7" t="n">
+        <v>6</v>
+      </c>
+      <c r="P6" s="7" t="n">
+        <v>150</v>
+      </c>
+      <c r="Q6" s="7" t="n">
+        <v>150</v>
+      </c>
+      <c r="R6" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="S6" s="7" t="n">
+        <v>42</v>
+      </c>
+      <c r="T6" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="U6" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="V6" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="W6" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="X6" s="7" t="n">
+        <v>0</v>
       </c>
       <c r="Y6" s="7" t="s">
         <v>108</v>
       </c>
-      <c r="Z6" s="7" t="s">
-        <v>108</v>
-      </c>
-      <c r="AA6" s="7" t="s">
-        <v>108</v>
-      </c>
-      <c r="AB6" s="7" t="s">
-        <v>114</v>
-      </c>
-      <c r="AC6" s="7" t="s">
-        <v>108</v>
+      <c r="Z6" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA6" s="7" t="n">
+        <v>125</v>
       </c>
     </row>
   </sheetData>

</xml_diff>